<commit_message>
update process flow and database document
</commit_message>
<xml_diff>
--- a/Documents/Database/Default Data.xlsx
+++ b/Documents/Database/Default Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>Tax in percentage</t>
+  </si>
+  <si>
+    <t>ROOM TRANSACTION</t>
   </si>
 </sst>
 </file>
@@ -349,6 +352,27 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -370,32 +394,11 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -410,14 +413,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:G11" totalsRowShown="0">
-  <autoFilter ref="B4:G11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:G13" totalsRowShown="0">
+  <autoFilter ref="B4:G13"/>
   <tableColumns count="6">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="code"/>
     <tableColumn id="3" name="status_type"/>
     <tableColumn id="4" name="name"/>
-    <tableColumn id="5" name="seq_num" dataDxfId="8"/>
+    <tableColumn id="5" name="seq_num" dataDxfId="6"/>
     <tableColumn id="6" name="descriptoin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -428,14 +431,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table35" displayName="Table35" ref="B4:I17" totalsRowShown="0">
   <autoFilter ref="B4:I17"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="id" dataDxfId="7"/>
+    <tableColumn id="1" name="id" dataDxfId="5"/>
     <tableColumn id="2" name="code"/>
     <tableColumn id="3" name="service_name"/>
     <tableColumn id="4" name="abbr"/>
-    <tableColumn id="5" name="is_include_tax" dataDxfId="6"/>
-    <tableColumn id="6" name="charge_amount" dataDxfId="5"/>
-    <tableColumn id="7" name="create_by" dataDxfId="4"/>
-    <tableColumn id="8" name="edit_by" dataDxfId="3"/>
+    <tableColumn id="5" name="is_include_tax" dataDxfId="4"/>
+    <tableColumn id="6" name="charge_amount" dataDxfId="3"/>
+    <tableColumn id="7" name="create_by" dataDxfId="2"/>
+    <tableColumn id="8" name="edit_by" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -445,7 +448,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356" displayName="Table356" ref="B4:E15" totalsRowShown="0">
   <autoFilter ref="B4:E15"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="id" dataDxfId="2"/>
+    <tableColumn id="1" name="id" dataDxfId="0"/>
     <tableColumn id="2" name="code"/>
     <tableColumn id="3" name="category_name"/>
     <tableColumn id="4" name="main_group"/>
@@ -767,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G11"/>
+  <dimension ref="B1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,6 +948,40 @@
       </c>
       <c r="F11" s="2">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1588,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>